<commit_message>
changement revue de code
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_dina.xlsx
+++ b/Fichiers equipe/revue_code_dina.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinaa\Documents\Maintenace Logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2084278\Documents\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78A5468-E006-41D9-9770-EC265D83D3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D179533-1A19-40FE-B1BA-899EDA097CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="1350" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,22 +605,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.69921875" customWidth="1"/>
-    <col min="4" max="4" width="70.3984375" customWidth="1"/>
-    <col min="5" max="5" width="15.69921875" customWidth="1"/>
-    <col min="6" max="6" width="18.296875" customWidth="1"/>
-    <col min="7" max="7" width="15.09765625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.850000000000001" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
@@ -631,7 +631,7 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>15</v>
       </c>
@@ -641,7 +641,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -653,7 +653,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -663,20 +663,20 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
@@ -684,7 +684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -707,7 +707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -724,7 +724,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>3</v>
       </c>
@@ -758,7 +758,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>4</v>
       </c>
@@ -775,7 +775,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>5</v>
       </c>
@@ -792,7 +792,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>6</v>
       </c>
@@ -809,7 +809,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>7</v>
       </c>
@@ -826,7 +826,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>8</v>
       </c>
@@ -843,24 +843,24 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>9</v>
       </c>
       <c r="B20" s="6">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>10</v>
       </c>
@@ -868,33 +868,31 @@
         <v>232</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>11</v>
       </c>
-      <c r="B22" s="6">
-        <v>232</v>
-      </c>
+      <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>12</v>
       </c>
@@ -911,7 +909,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>13</v>
       </c>
@@ -928,7 +926,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>14</v>
       </c>
@@ -945,7 +943,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>15</v>
       </c>
@@ -962,7 +960,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -971,7 +969,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="10"/>
       <c r="C28" s="4"/>
@@ -980,7 +978,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -989,7 +987,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -998,7 +996,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1007,7 +1005,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1016,7 +1014,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1025,7 +1023,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1034,7 +1032,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1043,7 +1041,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="2"/>
       <c r="C36" s="4"/>
@@ -1052,7 +1050,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1061,7 +1059,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1070,7 +1068,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39" s="9"/>
     </row>
   </sheetData>

</xml_diff>